<commit_message>
problem set 3 changes
</commit_message>
<xml_diff>
--- a/Module4/TimesheetCS5010.xlsx
+++ b/Module4/TimesheetCS5010.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Doyle</t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
     <t>Total Time On Task Q1 (minutes)</t>
   </si>
   <si>
@@ -110,6 +107,24 @@
   </si>
   <si>
     <t xml:space="preserve"> =========================committing to git: 2/7 14:56 =========================</t>
+  </si>
+  <si>
+    <t>Added tests for mouse events</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/8 9:21 =========================</t>
+  </si>
+  <si>
+    <t>More tests for mouse and key events</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/8 11:14 =========================</t>
+  </si>
+  <si>
+    <t>Got drag working better</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =========================committing to git: 2/8 13:15 =========================</t>
   </si>
 </sst>
 </file>
@@ -959,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,12 +1064,12 @@
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1093,12 +1108,12 @@
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1134,12 +1149,12 @@
         <v>60</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1166,120 +1181,222 @@
         <v>74</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41678</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>2</v>
+      </c>
+      <c r="I12" s="8">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>41678</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>2</v>
+      </c>
+      <c r="I14" s="8">
+        <f>60+12</f>
+        <v>72</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>41678</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.48819444444444443</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2</v>
+      </c>
+      <c r="I16" s="8">
+        <f>60+10</f>
+        <v>70</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="G21" s="4">
+        <f>SUMIF(G2:G20,"1",I2:I20)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="4">
-        <f>SUMIF(G3:G12,"1",I3:I12)</f>
+      <c r="G22" s="4">
+        <f>SUMIF(G3:G20,"2",I3:I20)</f>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="4">
+        <f>SUMIF(G3:G20,"3",I3:I20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="4">
+        <f>SUMIF(G3:G20,"4",I3:I20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="3">
+        <f>G13/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="3">
+        <f>G22/60</f>
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="3">
+        <f>G23/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="3">
+        <f>G24/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="4">
-        <f>SUMIF(G3:G12,"2",I3:I12)</f>
-        <v>239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="4">
-        <f>SUMIF(G3:G12,"3",I3:I12)</f>
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="4">
-        <f>SUMIF(G3:G12,"4",I3:I12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="3">
-        <f>G13/60</f>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="3">
-        <f>G14/60</f>
-        <v>3.9833333333333334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3">
-        <f>G15/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3">
-        <f>G16/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="G34" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="8">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="K34" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>